<commit_message>
neat stuff right.  Pretty mcuh done.  Just need proofreading n shit... and a new markov chain example pictre
</commit_message>
<xml_diff>
--- a/Book2 (Autosaved).xlsx
+++ b/Book2 (Autosaved).xlsx
@@ -15,12 +15,11 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027" iterateDelta="1E-4"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>Ai = 0.99</t>
   </si>
@@ -35,6 +34,33 @@
   </si>
   <si>
     <t>Ai = 0.9</t>
+  </si>
+  <si>
+    <t>ai = 0.999</t>
+  </si>
+  <si>
+    <t>wi = 0.2</t>
+  </si>
+  <si>
+    <t>ai = 0.99</t>
+  </si>
+  <si>
+    <t>ai= 0.99</t>
+  </si>
+  <si>
+    <t>wi = .2 around ~.45</t>
+  </si>
+  <si>
+    <t>starting money = 500</t>
+  </si>
+  <si>
+    <t>starting money = 1000</t>
+  </si>
+  <si>
+    <t>ai = 0.99 centered around ~.6</t>
+  </si>
+  <si>
+    <t>starting money = 1500</t>
   </si>
 </sst>
 </file>
@@ -70,8 +96,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -386,15 +413,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CV83"/>
+  <dimension ref="A1:CV173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A140" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E173" sqref="E173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="8.5703125"/>
+    <col min="1" max="2" width="8.5703125"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:100" x14ac:dyDescent="0.25">
@@ -2046,6 +2077,10 @@
         <f>_xlfn.STDEV.P(A17:AD17)</f>
         <v>1.1772380074428114E-2</v>
       </c>
+      <c r="C21">
+        <f>_xlfn.VAR.P(A17:AD17)</f>
+        <v>1.3858893261679207E-4</v>
+      </c>
     </row>
     <row r="22" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A22">
@@ -2056,6 +2091,10 @@
         <f>_xlfn.STDEV.P(A18:AD18)</f>
         <v>1.003885737727234E-2</v>
       </c>
+      <c r="C22">
+        <f t="shared" ref="C22:C24" si="0">_xlfn.VAR.P(A18:AD18)</f>
+        <v>1.0077865744121528E-4</v>
+      </c>
     </row>
     <row r="23" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A23">
@@ -2066,6 +2105,10 @@
         <f>_xlfn.STDEV.P(A19:AD19)</f>
         <v>8.5763897051820415E-3</v>
       </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>7.3554460375152504E-5</v>
+      </c>
     </row>
     <row r="24" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A24">
@@ -2076,6 +2119,10 @@
         <f>_xlfn.STDEV.P(A20:AD20)</f>
         <v>8.4254828130979412E-3</v>
       </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>7.0988760633808792E-5</v>
+      </c>
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A26">
@@ -2886,6 +2933,13 @@
         <f>_xlfn.STDEV.P(A38:AD38)</f>
         <v>7.7530854698423931E-3</v>
       </c>
+      <c r="C42">
+        <f>_xlfn.VAR.P(A38:AD38)</f>
+        <v>6.0110334302681246E-5</v>
+      </c>
+      <c r="E42">
+        <v>6.0110334302681199E-5</v>
+      </c>
     </row>
     <row r="43" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A43">
@@ -2896,6 +2950,13 @@
         <f>_xlfn.STDEV.P(A39:AD39)</f>
         <v>5.7894466909029149E-3</v>
       </c>
+      <c r="C43">
+        <f t="shared" ref="C43:C45" si="1">_xlfn.VAR.P(A39:AD39)</f>
+        <v>3.351769298680671E-5</v>
+      </c>
+      <c r="E43">
+        <v>3.3517692986806703E-5</v>
+      </c>
     </row>
     <row r="44" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A44">
@@ -2906,6 +2967,13 @@
         <f>_xlfn.STDEV.P(A40:AD40)</f>
         <v>4.4111784198907177E-3</v>
       </c>
+      <c r="C44">
+        <f t="shared" si="1"/>
+        <v>1.9458495052109565E-5</v>
+      </c>
+      <c r="E44">
+        <v>1.9458495052109599E-5</v>
+      </c>
     </row>
     <row r="45" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A45">
@@ -2916,6 +2984,13 @@
         <f>_xlfn.STDEV.P(A41:AD41)</f>
         <v>4.6740688821942386E-3</v>
       </c>
+      <c r="C45">
+        <f t="shared" si="1"/>
+        <v>2.1846919915496501E-5</v>
+      </c>
+      <c r="E45">
+        <v>2.1846919915496501E-5</v>
+      </c>
     </row>
     <row r="47" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
@@ -3302,6 +3377,10 @@
         <f>_xlfn.STDEV.P(A48:AD48)</f>
         <v>4.2082925836244428E-3</v>
       </c>
+      <c r="C52">
+        <f>_xlfn.VAR.P(A48:AD48)</f>
+        <v>1.770972646938849E-5</v>
+      </c>
     </row>
     <row r="53" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A53">
@@ -3312,6 +3391,10 @@
         <f>_xlfn.STDEV.P(A49:AD49)</f>
         <v>3.5667046290984773E-3</v>
       </c>
+      <c r="C53">
+        <f t="shared" ref="C53:C55" si="2">_xlfn.VAR.P(A49:AD49)</f>
+        <v>1.2721381911232506E-5</v>
+      </c>
     </row>
     <row r="54" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A54">
@@ -3322,6 +3405,10 @@
         <f>_xlfn.STDEV.P(A50:AD50)</f>
         <v>3.3724227721431302E-3</v>
       </c>
+      <c r="C54">
+        <f t="shared" si="2"/>
+        <v>1.1373235354069556E-5</v>
+      </c>
     </row>
     <row r="55" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A55">
@@ -3332,6 +3419,10 @@
         <f>_xlfn.STDEV.P(A51:AD51)</f>
         <v>4.018846911925944E-3</v>
       </c>
+      <c r="C55">
+        <f t="shared" si="2"/>
+        <v>1.6151130501496699E-5</v>
+      </c>
     </row>
     <row r="57" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
@@ -4571,7 +4662,7 @@
         <v>9.0216573149096417E-4</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A81">
         <f>AVERAGE(A77:AD77)</f>
         <v>0.87362076533512156</v>
@@ -4585,7 +4676,7 @@
         <v>7.8735833966823792E-4</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A82">
         <f>AVERAGE(A78:AD78)</f>
         <v>0.90295952531106038</v>
@@ -4599,7 +4690,7 @@
         <v>5.3790189442213328E-4</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A83">
         <f>AVERAGE(A79:AD79)</f>
         <v>0.87776783332288799</v>
@@ -4611,6 +4702,2995 @@
       <c r="C83">
         <f>VAR(A79:AD79)</f>
         <v>9.376236903241023E-4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>0.78570311390259795</v>
+      </c>
+      <c r="B85">
+        <v>0.79009248858173597</v>
+      </c>
+      <c r="C85">
+        <v>0.78580292924867001</v>
+      </c>
+      <c r="D85">
+        <v>0.79935978896746995</v>
+      </c>
+      <c r="E85">
+        <v>0.79123551062076802</v>
+      </c>
+      <c r="F85">
+        <v>0.78709093420749698</v>
+      </c>
+      <c r="G85">
+        <v>0.78611622700318995</v>
+      </c>
+      <c r="H85">
+        <v>0.78505649633566199</v>
+      </c>
+      <c r="I85">
+        <v>0.79373485541033695</v>
+      </c>
+      <c r="J85">
+        <v>0.78935948548314505</v>
+      </c>
+      <c r="K85">
+        <v>0.78930908286725399</v>
+      </c>
+      <c r="L85">
+        <v>0.78787842657766805</v>
+      </c>
+      <c r="M85">
+        <v>0.79579496625249302</v>
+      </c>
+      <c r="N85">
+        <v>0.79060691657063098</v>
+      </c>
+      <c r="O85">
+        <v>0.78956268540306396</v>
+      </c>
+      <c r="P85">
+        <v>0.78875825482717499</v>
+      </c>
+      <c r="Q85">
+        <v>0.78595312539798001</v>
+      </c>
+      <c r="R85">
+        <v>0.79179326407356598</v>
+      </c>
+      <c r="S85">
+        <v>0.78400612265583902</v>
+      </c>
+      <c r="T85">
+        <v>0.78640657222219801</v>
+      </c>
+      <c r="U85">
+        <v>0.788330846560098</v>
+      </c>
+      <c r="V85">
+        <v>0.78678895673058702</v>
+      </c>
+      <c r="W85">
+        <v>0.78455774575710502</v>
+      </c>
+      <c r="X85">
+        <v>0.79862947202136703</v>
+      </c>
+      <c r="Y85">
+        <v>0.79046955892889803</v>
+      </c>
+      <c r="Z85">
+        <v>0.78092598877450403</v>
+      </c>
+      <c r="AA85">
+        <v>0.79351208592579103</v>
+      </c>
+      <c r="AB85">
+        <v>0.79565876157745097</v>
+      </c>
+      <c r="AC85">
+        <v>0.79538293303579799</v>
+      </c>
+      <c r="AD85">
+        <v>0.79672182457080698</v>
+      </c>
+    </row>
+    <row r="86" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>0.86055083790764497</v>
+      </c>
+      <c r="B86">
+        <v>0.86504220124659004</v>
+      </c>
+      <c r="C86">
+        <v>0.86344594358444104</v>
+      </c>
+      <c r="D86">
+        <v>0.863466649269366</v>
+      </c>
+      <c r="E86">
+        <v>0.86437082617053196</v>
+      </c>
+      <c r="F86">
+        <v>0.86631765802241001</v>
+      </c>
+      <c r="G86">
+        <v>0.86738379319245495</v>
+      </c>
+      <c r="H86">
+        <v>0.86089869116947404</v>
+      </c>
+      <c r="I86">
+        <v>0.86233970830023199</v>
+      </c>
+      <c r="J86">
+        <v>0.86306121856514895</v>
+      </c>
+      <c r="K86">
+        <v>0.86603516556068505</v>
+      </c>
+      <c r="L86">
+        <v>0.86046803979359998</v>
+      </c>
+      <c r="M86">
+        <v>0.860751088470323</v>
+      </c>
+      <c r="N86">
+        <v>0.86382066478792496</v>
+      </c>
+      <c r="O86">
+        <v>0.86499109320112</v>
+      </c>
+      <c r="P86">
+        <v>0.85950158451351699</v>
+      </c>
+      <c r="Q86">
+        <v>0.86499838237869398</v>
+      </c>
+      <c r="R86">
+        <v>0.86327994094721505</v>
+      </c>
+      <c r="S86">
+        <v>0.86148810688340705</v>
+      </c>
+      <c r="T86">
+        <v>0.86501844316028897</v>
+      </c>
+      <c r="U86">
+        <v>0.86195361946784999</v>
+      </c>
+      <c r="V86">
+        <v>0.86322769027643398</v>
+      </c>
+      <c r="W86">
+        <v>0.863415408575544</v>
+      </c>
+      <c r="X86">
+        <v>0.86332298303944099</v>
+      </c>
+      <c r="Y86">
+        <v>0.86086247881794198</v>
+      </c>
+      <c r="Z86">
+        <v>0.86035594307605401</v>
+      </c>
+      <c r="AA86">
+        <v>0.86786574055487598</v>
+      </c>
+      <c r="AB86">
+        <v>0.85995048148188602</v>
+      </c>
+      <c r="AC86">
+        <v>0.86767157741754097</v>
+      </c>
+      <c r="AD86">
+        <v>0.86339438726692797</v>
+      </c>
+    </row>
+    <row r="87" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>0.889014332016826</v>
+      </c>
+      <c r="B87">
+        <v>0.88924699640035998</v>
+      </c>
+      <c r="C87">
+        <v>0.88795623260058698</v>
+      </c>
+      <c r="D87">
+        <v>0.88891958081431899</v>
+      </c>
+      <c r="E87">
+        <v>0.88784234631070402</v>
+      </c>
+      <c r="F87">
+        <v>0.887746402401142</v>
+      </c>
+      <c r="G87">
+        <v>0.88658294413095096</v>
+      </c>
+      <c r="H87">
+        <v>0.88710578981093502</v>
+      </c>
+      <c r="I87">
+        <v>0.889662359184754</v>
+      </c>
+      <c r="J87">
+        <v>0.88854011769274599</v>
+      </c>
+      <c r="K87">
+        <v>0.88527659333358399</v>
+      </c>
+      <c r="L87">
+        <v>0.89105102108995904</v>
+      </c>
+      <c r="M87">
+        <v>0.88457284272012005</v>
+      </c>
+      <c r="N87">
+        <v>0.89071728485120505</v>
+      </c>
+      <c r="O87">
+        <v>0.88921616798686698</v>
+      </c>
+      <c r="P87">
+        <v>0.88740456008567203</v>
+      </c>
+      <c r="Q87">
+        <v>0.88906491062922199</v>
+      </c>
+      <c r="R87">
+        <v>0.88962305513654105</v>
+      </c>
+      <c r="S87">
+        <v>0.89041532085025898</v>
+      </c>
+      <c r="T87">
+        <v>0.89014892668586099</v>
+      </c>
+      <c r="U87">
+        <v>0.88745184378535802</v>
+      </c>
+      <c r="V87">
+        <v>0.885958163825044</v>
+      </c>
+      <c r="W87">
+        <v>0.88400195954799499</v>
+      </c>
+      <c r="X87">
+        <v>0.88327993530285598</v>
+      </c>
+      <c r="Y87">
+        <v>0.89020955446440098</v>
+      </c>
+      <c r="Z87">
+        <v>0.88801062081656201</v>
+      </c>
+      <c r="AA87">
+        <v>0.88407427459163201</v>
+      </c>
+      <c r="AB87">
+        <v>0.88970862834082998</v>
+      </c>
+      <c r="AC87">
+        <v>0.88472460374662898</v>
+      </c>
+      <c r="AD87">
+        <v>0.88893447224959998</v>
+      </c>
+    </row>
+    <row r="88" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>0.86431339922320705</v>
+      </c>
+      <c r="B88">
+        <v>0.86440833202359202</v>
+      </c>
+      <c r="C88">
+        <v>0.86313103528869395</v>
+      </c>
+      <c r="D88">
+        <v>0.86343508672681701</v>
+      </c>
+      <c r="E88">
+        <v>0.86346787561831195</v>
+      </c>
+      <c r="F88">
+        <v>0.867778878804493</v>
+      </c>
+      <c r="G88">
+        <v>0.85703833666654605</v>
+      </c>
+      <c r="H88">
+        <v>0.86051028745474101</v>
+      </c>
+      <c r="I88">
+        <v>0.86199961568652395</v>
+      </c>
+      <c r="J88">
+        <v>0.857867206591723</v>
+      </c>
+      <c r="K88">
+        <v>0.858922007119856</v>
+      </c>
+      <c r="L88">
+        <v>0.85944649076064605</v>
+      </c>
+      <c r="M88">
+        <v>0.86118838816560295</v>
+      </c>
+      <c r="N88">
+        <v>0.86095649935993002</v>
+      </c>
+      <c r="O88">
+        <v>0.86433360897743305</v>
+      </c>
+      <c r="P88">
+        <v>0.86387253154628196</v>
+      </c>
+      <c r="Q88">
+        <v>0.86632730983028905</v>
+      </c>
+      <c r="R88">
+        <v>0.86243196073011497</v>
+      </c>
+      <c r="S88">
+        <v>0.86555245333354103</v>
+      </c>
+      <c r="T88">
+        <v>0.86423719915853603</v>
+      </c>
+      <c r="U88">
+        <v>0.86265434729811596</v>
+      </c>
+      <c r="V88">
+        <v>0.85998756862084103</v>
+      </c>
+      <c r="W88">
+        <v>0.86076875276259601</v>
+      </c>
+      <c r="X88">
+        <v>0.859602642166305</v>
+      </c>
+      <c r="Y88">
+        <v>0.86578406037037903</v>
+      </c>
+      <c r="Z88">
+        <v>0.86163664377056104</v>
+      </c>
+      <c r="AA88">
+        <v>0.86316212683959004</v>
+      </c>
+      <c r="AB88">
+        <v>0.85733214069475705</v>
+      </c>
+      <c r="AC88">
+        <v>0.85620192679197704</v>
+      </c>
+      <c r="AD88">
+        <v>0.86107776295930805</v>
+      </c>
+    </row>
+    <row r="89" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <f>AVERAGE(A85:AD85)</f>
+        <v>0.78981998068304493</v>
+      </c>
+      <c r="B89">
+        <f>_xlfn.STDEV.P(A85:AD85)</f>
+        <v>4.5237932421641159E-3</v>
+      </c>
+      <c r="C89">
+        <f>_xlfn.VAR.P(A85:AD85)</f>
+        <v>2.0464705297849721E-5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <f t="shared" ref="A90:A92" si="3">AVERAGE(A86:AD86)</f>
+        <v>0.86330834490331909</v>
+      </c>
+      <c r="B90">
+        <f t="shared" ref="B90:B92" si="4">_xlfn.STDEV.P(A86:AD86)</f>
+        <v>2.31386681159015E-3</v>
+      </c>
+      <c r="C90">
+        <f t="shared" ref="C90:C92" si="5">_xlfn.VAR.P(A86:AD86)</f>
+        <v>5.3539796217783669E-6</v>
+      </c>
+    </row>
+    <row r="91" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <f t="shared" si="3"/>
+        <v>0.88788206138011716</v>
+      </c>
+      <c r="B91">
+        <f>_xlfn.STDEV.P(A87:AD87)</f>
+        <v>2.1480362757524351E-3</v>
+      </c>
+      <c r="C91">
+        <f t="shared" si="5"/>
+        <v>4.6140598419483914E-6</v>
+      </c>
+    </row>
+    <row r="92" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <f t="shared" si="3"/>
+        <v>0.86198088251137706</v>
+      </c>
+      <c r="B92">
+        <f t="shared" si="4"/>
+        <v>2.834187201334889E-3</v>
+      </c>
+      <c r="C92">
+        <f t="shared" si="5"/>
+        <v>8.0326170922104916E-6</v>
+      </c>
+    </row>
+    <row r="95" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>8</v>
+      </c>
+      <c r="B95" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="96" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>0.82451137552339004</v>
+      </c>
+      <c r="B96">
+        <v>0.823170097438918</v>
+      </c>
+      <c r="C96">
+        <v>0.82315376957154596</v>
+      </c>
+      <c r="D96">
+        <v>0.82381093581083897</v>
+      </c>
+      <c r="E96">
+        <v>0.82449096903564001</v>
+      </c>
+      <c r="F96">
+        <v>0.82274351748045005</v>
+      </c>
+      <c r="G96">
+        <v>0.82671146523050598</v>
+      </c>
+      <c r="H96">
+        <v>0.82461602589553196</v>
+      </c>
+      <c r="I96">
+        <v>0.82430104854777198</v>
+      </c>
+      <c r="J96">
+        <v>0.82282877012275102</v>
+      </c>
+      <c r="K96">
+        <v>0.82365965317357703</v>
+      </c>
+      <c r="L96">
+        <v>0.82446809664458198</v>
+      </c>
+      <c r="M96">
+        <v>0.824831828298347</v>
+      </c>
+      <c r="N96">
+        <v>0.82528022641520904</v>
+      </c>
+      <c r="O96">
+        <v>0.82446152827949004</v>
+      </c>
+      <c r="P96">
+        <v>0.82301464844254502</v>
+      </c>
+      <c r="Q96">
+        <v>0.822171219542014</v>
+      </c>
+      <c r="R96">
+        <v>0.82381115176759701</v>
+      </c>
+      <c r="S96">
+        <v>0.82352547477252103</v>
+      </c>
+      <c r="T96">
+        <v>0.82328044807887801</v>
+      </c>
+      <c r="U96">
+        <v>0.82170340870493397</v>
+      </c>
+      <c r="V96">
+        <v>0.82588769008942198</v>
+      </c>
+      <c r="W96">
+        <v>0.82407166458427505</v>
+      </c>
+      <c r="X96">
+        <v>0.82259405974069499</v>
+      </c>
+      <c r="Y96">
+        <v>0.82302199913747898</v>
+      </c>
+      <c r="Z96">
+        <v>0.82297261828861701</v>
+      </c>
+      <c r="AA96">
+        <v>0.82238543888131899</v>
+      </c>
+      <c r="AB96">
+        <v>0.82374241542069704</v>
+      </c>
+      <c r="AC96">
+        <v>0.82291477280052305</v>
+      </c>
+      <c r="AD96">
+        <v>0.82331499005175801</v>
+      </c>
+    </row>
+    <row r="97" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>0.89902872751283103</v>
+      </c>
+      <c r="B97">
+        <v>0.89549274648672705</v>
+      </c>
+      <c r="C97">
+        <v>0.89803169397471205</v>
+      </c>
+      <c r="D97">
+        <v>0.89903719971294505</v>
+      </c>
+      <c r="E97">
+        <v>0.89661574709640002</v>
+      </c>
+      <c r="F97">
+        <v>0.89996390719351504</v>
+      </c>
+      <c r="G97">
+        <v>0.89895015674197398</v>
+      </c>
+      <c r="H97">
+        <v>0.89719291652348399</v>
+      </c>
+      <c r="I97">
+        <v>0.89863421565815305</v>
+      </c>
+      <c r="J97">
+        <v>0.89789250808656496</v>
+      </c>
+      <c r="K97">
+        <v>0.895340367020654</v>
+      </c>
+      <c r="L97">
+        <v>0.90059786118253005</v>
+      </c>
+      <c r="M97">
+        <v>0.89711536124472302</v>
+      </c>
+      <c r="N97">
+        <v>0.897636082692992</v>
+      </c>
+      <c r="O97">
+        <v>0.89905639602925802</v>
+      </c>
+      <c r="P97">
+        <v>0.89899431612246905</v>
+      </c>
+      <c r="Q97">
+        <v>0.89718929510688095</v>
+      </c>
+      <c r="R97">
+        <v>0.89802412505527596</v>
+      </c>
+      <c r="S97">
+        <v>0.89766653123085804</v>
+      </c>
+      <c r="T97">
+        <v>0.89770157808862105</v>
+      </c>
+      <c r="U97">
+        <v>0.90054337265814099</v>
+      </c>
+      <c r="V97">
+        <v>0.897961170215691</v>
+      </c>
+      <c r="W97">
+        <v>0.89623730935073997</v>
+      </c>
+      <c r="X97">
+        <v>0.89932736505072697</v>
+      </c>
+      <c r="Y97">
+        <v>0.89801754243816201</v>
+      </c>
+      <c r="Z97">
+        <v>0.89615087963236795</v>
+      </c>
+      <c r="AA97">
+        <v>0.89895825082671199</v>
+      </c>
+      <c r="AB97">
+        <v>0.89766551838959896</v>
+      </c>
+      <c r="AC97">
+        <v>0.89955069501990503</v>
+      </c>
+      <c r="AD97">
+        <v>0.90012531593757705</v>
+      </c>
+    </row>
+    <row r="98" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>0.924089486036481</v>
+      </c>
+      <c r="B98">
+        <v>0.92379510969643297</v>
+      </c>
+      <c r="C98">
+        <v>0.923395581486256</v>
+      </c>
+      <c r="D98">
+        <v>0.927927209900971</v>
+      </c>
+      <c r="E98">
+        <v>0.92347112429495304</v>
+      </c>
+      <c r="F98">
+        <v>0.92405692399270001</v>
+      </c>
+      <c r="G98">
+        <v>0.92663705383350503</v>
+      </c>
+      <c r="H98">
+        <v>0.92534895069297696</v>
+      </c>
+      <c r="I98">
+        <v>0.924637222782278</v>
+      </c>
+      <c r="J98">
+        <v>0.92480498980766501</v>
+      </c>
+      <c r="K98">
+        <v>0.92527708166854195</v>
+      </c>
+      <c r="L98">
+        <v>0.92316808507166104</v>
+      </c>
+      <c r="M98">
+        <v>0.92440878812890104</v>
+      </c>
+      <c r="N98">
+        <v>0.92472119279803799</v>
+      </c>
+      <c r="O98">
+        <v>0.92463365735975001</v>
+      </c>
+      <c r="P98">
+        <v>0.92496606006461801</v>
+      </c>
+      <c r="Q98">
+        <v>0.92451123248771705</v>
+      </c>
+      <c r="R98">
+        <v>0.92609201701001098</v>
+      </c>
+      <c r="S98">
+        <v>0.92475927586109796</v>
+      </c>
+      <c r="T98">
+        <v>0.92390913442170297</v>
+      </c>
+      <c r="U98">
+        <v>0.92410796099635795</v>
+      </c>
+      <c r="V98">
+        <v>0.92616665513547403</v>
+      </c>
+      <c r="W98">
+        <v>0.92523775751475801</v>
+      </c>
+      <c r="X98">
+        <v>0.92436798083821803</v>
+      </c>
+      <c r="Y98">
+        <v>0.92474570309608295</v>
+      </c>
+      <c r="Z98">
+        <v>0.92424765921489305</v>
+      </c>
+      <c r="AA98">
+        <v>0.923335875670661</v>
+      </c>
+      <c r="AB98">
+        <v>0.92488346240158503</v>
+      </c>
+      <c r="AC98">
+        <v>0.92328083063403599</v>
+      </c>
+      <c r="AD98">
+        <v>0.92418729270290201</v>
+      </c>
+    </row>
+    <row r="99" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>0.90015809918047596</v>
+      </c>
+      <c r="B99">
+        <v>0.89828835938497098</v>
+      </c>
+      <c r="C99">
+        <v>0.89869457462286195</v>
+      </c>
+      <c r="D99">
+        <v>0.89785272795711002</v>
+      </c>
+      <c r="E99">
+        <v>0.89756771791040602</v>
+      </c>
+      <c r="F99">
+        <v>0.89661727708657202</v>
+      </c>
+      <c r="G99">
+        <v>0.89897685050354104</v>
+      </c>
+      <c r="H99">
+        <v>0.89646751325920304</v>
+      </c>
+      <c r="I99">
+        <v>0.89769043813397298</v>
+      </c>
+      <c r="J99">
+        <v>0.89869151417216597</v>
+      </c>
+      <c r="K99">
+        <v>0.89881038136472702</v>
+      </c>
+      <c r="L99">
+        <v>0.89965254821839402</v>
+      </c>
+      <c r="M99">
+        <v>0.89803826736240699</v>
+      </c>
+      <c r="N99">
+        <v>0.89827536128673302</v>
+      </c>
+      <c r="O99">
+        <v>0.89811653746852305</v>
+      </c>
+      <c r="P99">
+        <v>0.89854219500252297</v>
+      </c>
+      <c r="Q99">
+        <v>0.89874344280433605</v>
+      </c>
+      <c r="R99">
+        <v>0.90037482542824099</v>
+      </c>
+      <c r="S99">
+        <v>0.89807153406038698</v>
+      </c>
+      <c r="T99">
+        <v>0.90057612930147901</v>
+      </c>
+      <c r="U99">
+        <v>0.89845142684314805</v>
+      </c>
+      <c r="V99">
+        <v>0.90126243695457797</v>
+      </c>
+      <c r="W99">
+        <v>0.89757342610581203</v>
+      </c>
+      <c r="X99">
+        <v>0.90026426948637195</v>
+      </c>
+      <c r="Y99">
+        <v>0.89940839564722197</v>
+      </c>
+      <c r="Z99">
+        <v>0.89755769358274495</v>
+      </c>
+      <c r="AA99">
+        <v>0.89765935172550804</v>
+      </c>
+      <c r="AB99">
+        <v>0.89693557412973302</v>
+      </c>
+      <c r="AC99">
+        <v>0.89773748257329999</v>
+      </c>
+      <c r="AD99">
+        <v>0.89961778777071999</v>
+      </c>
+    </row>
+    <row r="100" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <f>AVERAGE(A96:AD96)</f>
+        <v>0.82371504359239411</v>
+      </c>
+      <c r="B100">
+        <f>_xlfn.STDEV.P(A96:AD96)</f>
+        <v>1.0863436756453062E-3</v>
+      </c>
+      <c r="C100">
+        <f>_xlfn.VAR.P(A96:AD96)</f>
+        <v>1.1801425816145541E-6</v>
+      </c>
+    </row>
+    <row r="101" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <f t="shared" ref="A101:A103" si="6">AVERAGE(A97:AD97)</f>
+        <v>0.8981566384093731</v>
+      </c>
+      <c r="B101">
+        <f t="shared" ref="B101:B103" si="7">_xlfn.STDEV.P(A97:AD97)</f>
+        <v>1.3642723577265803E-3</v>
+      </c>
+      <c r="C101">
+        <f t="shared" ref="C101:C103" si="8">_xlfn.VAR.P(A97:AD97)</f>
+        <v>1.8612390660568424E-6</v>
+      </c>
+    </row>
+    <row r="102" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <f t="shared" si="6"/>
+        <v>0.92463904518670748</v>
+      </c>
+      <c r="B102">
+        <f>_xlfn.STDEV.P(A98:AD98)</f>
+        <v>1.0332813337488578E-3</v>
+      </c>
+      <c r="C102">
+        <f t="shared" si="8"/>
+        <v>1.0676703146738184E-6</v>
+      </c>
+    </row>
+    <row r="103" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <f>AVERAGE(A99:AD99)</f>
+        <v>0.89855580464427243</v>
+      </c>
+      <c r="B103">
+        <f t="shared" si="7"/>
+        <v>1.1666158790171709E-3</v>
+      </c>
+      <c r="C103">
+        <f t="shared" si="8"/>
+        <v>1.3609926091750061E-6</v>
+      </c>
+    </row>
+    <row r="107" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>0.820888294049823</v>
+      </c>
+      <c r="B107">
+        <v>0.819726746502073</v>
+      </c>
+      <c r="C107">
+        <v>0.81712184810129296</v>
+      </c>
+      <c r="D107">
+        <v>0.82455424985471903</v>
+      </c>
+      <c r="E107">
+        <v>0.82300280310667595</v>
+      </c>
+      <c r="F107">
+        <v>0.817047803077251</v>
+      </c>
+      <c r="G107">
+        <v>0.82429499167978204</v>
+      </c>
+      <c r="H107">
+        <v>0.82269305488270605</v>
+      </c>
+      <c r="I107">
+        <v>0.81631261896260299</v>
+      </c>
+      <c r="J107">
+        <v>0.81718631976552003</v>
+      </c>
+      <c r="K107">
+        <v>0.82531743370017996</v>
+      </c>
+      <c r="L107">
+        <v>0.82271451684880004</v>
+      </c>
+      <c r="M107">
+        <v>0.82196111280620299</v>
+      </c>
+      <c r="N107">
+        <v>0.817535214868648</v>
+      </c>
+      <c r="O107">
+        <v>0.81888328916084796</v>
+      </c>
+      <c r="P107">
+        <v>0.82169058603147505</v>
+      </c>
+      <c r="Q107">
+        <v>0.82020323028232001</v>
+      </c>
+      <c r="R107">
+        <v>0.82798263949904904</v>
+      </c>
+      <c r="S107">
+        <v>0.82186772493557902</v>
+      </c>
+      <c r="T107">
+        <v>0.82647008377945796</v>
+      </c>
+      <c r="U107">
+        <v>0.82315455514999603</v>
+      </c>
+      <c r="V107">
+        <v>0.81458663123337804</v>
+      </c>
+      <c r="W107">
+        <v>0.82185023641793797</v>
+      </c>
+      <c r="X107">
+        <v>0.82325348325653502</v>
+      </c>
+      <c r="Y107">
+        <v>0.82166416280271404</v>
+      </c>
+      <c r="Z107">
+        <v>0.81794397974035504</v>
+      </c>
+      <c r="AA107">
+        <v>0.82074137960383498</v>
+      </c>
+      <c r="AB107">
+        <v>0.82317198466239005</v>
+      </c>
+      <c r="AC107">
+        <v>0.81881600198910898</v>
+      </c>
+      <c r="AD107">
+        <v>0.81521255640215096</v>
+      </c>
+    </row>
+    <row r="108" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>0.90129502743116796</v>
+      </c>
+      <c r="B108">
+        <v>0.89825201658682197</v>
+      </c>
+      <c r="C108">
+        <v>0.90463102439173004</v>
+      </c>
+      <c r="D108">
+        <v>0.89833620307387296</v>
+      </c>
+      <c r="E108">
+        <v>0.899698704083018</v>
+      </c>
+      <c r="F108">
+        <v>0.89943800209318603</v>
+      </c>
+      <c r="G108">
+        <v>0.90204605057920395</v>
+      </c>
+      <c r="H108">
+        <v>0.897466919908953</v>
+      </c>
+      <c r="I108">
+        <v>0.89995860952370699</v>
+      </c>
+      <c r="J108">
+        <v>0.89803005877043995</v>
+      </c>
+      <c r="K108">
+        <v>0.89603309481306403</v>
+      </c>
+      <c r="L108">
+        <v>0.90098394300154305</v>
+      </c>
+      <c r="M108">
+        <v>0.891652154731158</v>
+      </c>
+      <c r="N108">
+        <v>0.90340085858072705</v>
+      </c>
+      <c r="O108">
+        <v>0.90034389629424805</v>
+      </c>
+      <c r="P108">
+        <v>0.90107082814616701</v>
+      </c>
+      <c r="Q108">
+        <v>0.89821072622207798</v>
+      </c>
+      <c r="R108">
+        <v>0.90185540454905899</v>
+      </c>
+      <c r="S108">
+        <v>0.89759167994477795</v>
+      </c>
+      <c r="T108">
+        <v>0.90001080732006</v>
+      </c>
+      <c r="U108">
+        <v>0.89202799127228904</v>
+      </c>
+      <c r="V108">
+        <v>0.89549782027667801</v>
+      </c>
+      <c r="W108">
+        <v>0.89894934990859998</v>
+      </c>
+      <c r="X108">
+        <v>0.89779756739944006</v>
+      </c>
+      <c r="Y108">
+        <v>0.89862215128680101</v>
+      </c>
+      <c r="Z108">
+        <v>0.89566309956378298</v>
+      </c>
+      <c r="AA108">
+        <v>0.89370475643872005</v>
+      </c>
+      <c r="AB108">
+        <v>0.90009663367632298</v>
+      </c>
+      <c r="AC108">
+        <v>0.89951741731246204</v>
+      </c>
+      <c r="AD108">
+        <v>0.90016425172303904</v>
+      </c>
+    </row>
+    <row r="109" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>0.92343946634861096</v>
+      </c>
+      <c r="B109">
+        <v>0.91781698092505104</v>
+      </c>
+      <c r="C109">
+        <v>0.92167987462471801</v>
+      </c>
+      <c r="D109">
+        <v>0.92476567393888898</v>
+      </c>
+      <c r="E109">
+        <v>0.920694982555888</v>
+      </c>
+      <c r="F109">
+        <v>0.92678061306708803</v>
+      </c>
+      <c r="G109">
+        <v>0.91963338405293305</v>
+      </c>
+      <c r="H109">
+        <v>0.92167169473586597</v>
+      </c>
+      <c r="I109">
+        <v>0.92564456356952496</v>
+      </c>
+      <c r="J109">
+        <v>0.92371888680013103</v>
+      </c>
+      <c r="K109">
+        <v>0.93355101963940401</v>
+      </c>
+      <c r="L109">
+        <v>0.92139972572617101</v>
+      </c>
+      <c r="M109">
+        <v>0.92771551380866701</v>
+      </c>
+      <c r="N109">
+        <v>0.93175101576300201</v>
+      </c>
+      <c r="O109">
+        <v>0.93162371461937199</v>
+      </c>
+      <c r="P109">
+        <v>0.925429897949966</v>
+      </c>
+      <c r="Q109">
+        <v>0.92299225698140797</v>
+      </c>
+      <c r="R109">
+        <v>0.93004577198038896</v>
+      </c>
+      <c r="S109">
+        <v>0.92904029764141305</v>
+      </c>
+      <c r="T109">
+        <v>0.93022018051018296</v>
+      </c>
+      <c r="U109">
+        <v>0.92403575048807296</v>
+      </c>
+      <c r="V109">
+        <v>0.92626745936585597</v>
+      </c>
+      <c r="W109">
+        <v>0.92880255738975703</v>
+      </c>
+      <c r="X109">
+        <v>0.922799618706314</v>
+      </c>
+      <c r="Y109">
+        <v>0.92783113237214498</v>
+      </c>
+      <c r="Z109">
+        <v>0.92754928502202605</v>
+      </c>
+      <c r="AA109">
+        <v>0.926422234773006</v>
+      </c>
+      <c r="AB109">
+        <v>0.92274860738936104</v>
+      </c>
+      <c r="AC109">
+        <v>0.92201237784011203</v>
+      </c>
+      <c r="AD109">
+        <v>0.924038390253624</v>
+      </c>
+    </row>
+    <row r="110" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>0.89441674671636695</v>
+      </c>
+      <c r="B110">
+        <v>0.89860293455413198</v>
+      </c>
+      <c r="C110">
+        <v>0.90438822676309205</v>
+      </c>
+      <c r="D110">
+        <v>0.90098496729136901</v>
+      </c>
+      <c r="E110">
+        <v>0.90818402908817997</v>
+      </c>
+      <c r="F110">
+        <v>0.90139369731394703</v>
+      </c>
+      <c r="G110">
+        <v>0.89619066852278095</v>
+      </c>
+      <c r="H110">
+        <v>0.89968280093534403</v>
+      </c>
+      <c r="I110">
+        <v>0.90471446155775703</v>
+      </c>
+      <c r="J110">
+        <v>0.89666860713619001</v>
+      </c>
+      <c r="K110">
+        <v>0.89164208887329599</v>
+      </c>
+      <c r="L110">
+        <v>0.90557599757961105</v>
+      </c>
+      <c r="M110">
+        <v>0.90584394923095501</v>
+      </c>
+      <c r="N110">
+        <v>0.89892071507566895</v>
+      </c>
+      <c r="O110">
+        <v>0.896565237778983</v>
+      </c>
+      <c r="P110">
+        <v>0.89782900692134804</v>
+      </c>
+      <c r="Q110">
+        <v>0.90020952259887399</v>
+      </c>
+      <c r="R110">
+        <v>0.89789032556204296</v>
+      </c>
+      <c r="S110">
+        <v>0.902116260851901</v>
+      </c>
+      <c r="T110">
+        <v>0.89677651556876503</v>
+      </c>
+      <c r="U110">
+        <v>0.89924240514616305</v>
+      </c>
+      <c r="V110">
+        <v>0.90368343440731302</v>
+      </c>
+      <c r="W110">
+        <v>0.90011818191301496</v>
+      </c>
+      <c r="X110">
+        <v>0.90216211299983096</v>
+      </c>
+      <c r="Y110">
+        <v>0.894671889742641</v>
+      </c>
+      <c r="Z110">
+        <v>0.90480796341912495</v>
+      </c>
+      <c r="AA110">
+        <v>0.90174760635534001</v>
+      </c>
+      <c r="AB110">
+        <v>0.90281188136804602</v>
+      </c>
+      <c r="AC110">
+        <v>0.899893075779723</v>
+      </c>
+      <c r="AD110">
+        <v>0.89829071614972</v>
+      </c>
+    </row>
+    <row r="111" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <f>AVERAGE(A107:AD107)</f>
+        <v>0.82092831777178044</v>
+      </c>
+      <c r="B111">
+        <f>_xlfn.STDEV.P(A107:AD107)</f>
+        <v>3.2810494738963469E-3</v>
+      </c>
+      <c r="C111">
+        <f>_xlfn.VAR.P(A107:AD107)</f>
+        <v>1.0765285650155496E-5</v>
+      </c>
+    </row>
+    <row r="112" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <f t="shared" ref="A112:A114" si="9">AVERAGE(A108:AD108)</f>
+        <v>0.89874490163010423</v>
+      </c>
+      <c r="B112">
+        <f t="shared" ref="B112:B114" si="10">_xlfn.STDEV.P(A108:AD108)</f>
+        <v>2.9361557964713561E-3</v>
+      </c>
+      <c r="C112">
+        <f t="shared" ref="C112:C114" si="11">_xlfn.VAR.P(A108:AD108)</f>
+        <v>8.6210108611523444E-6</v>
+      </c>
+    </row>
+    <row r="113" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <f t="shared" si="9"/>
+        <v>0.92540409762796516</v>
+      </c>
+      <c r="B113">
+        <f t="shared" si="10"/>
+        <v>3.8004310152487258E-3</v>
+      </c>
+      <c r="C113">
+        <f t="shared" si="11"/>
+        <v>1.4443275901664463E-5</v>
+      </c>
+    </row>
+    <row r="114" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <f t="shared" si="9"/>
+        <v>0.90020086757338391</v>
+      </c>
+      <c r="B114">
+        <f t="shared" si="10"/>
+        <v>3.7654783106876584E-3</v>
+      </c>
+      <c r="C114">
+        <f t="shared" si="11"/>
+        <v>1.4178826908259181E-5</v>
+      </c>
+    </row>
+    <row r="118" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>7</v>
+      </c>
+      <c r="B118" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="119" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>0.43041124642600498</v>
+      </c>
+      <c r="B119">
+        <v>0.43014116545820102</v>
+      </c>
+      <c r="C119">
+        <v>0.42733593934804998</v>
+      </c>
+      <c r="D119">
+        <v>0.42186148359233999</v>
+      </c>
+      <c r="E119">
+        <v>0.43231052974332801</v>
+      </c>
+      <c r="F119">
+        <v>0.42411641600848499</v>
+      </c>
+      <c r="G119">
+        <v>0.42750634833031897</v>
+      </c>
+      <c r="H119">
+        <v>0.41778648947458402</v>
+      </c>
+      <c r="I119">
+        <v>0.42906433595686799</v>
+      </c>
+      <c r="J119">
+        <v>0.42566328598831998</v>
+      </c>
+      <c r="K119">
+        <v>0.43478832622282698</v>
+      </c>
+      <c r="L119">
+        <v>0.42897869249018</v>
+      </c>
+      <c r="M119">
+        <v>0.429474385847744</v>
+      </c>
+      <c r="N119">
+        <v>0.43127344050920602</v>
+      </c>
+      <c r="O119">
+        <v>0.43082804155920601</v>
+      </c>
+      <c r="P119">
+        <v>0.43049630823095802</v>
+      </c>
+      <c r="Q119">
+        <v>0.42744571075639198</v>
+      </c>
+      <c r="R119">
+        <v>0.42481088014729901</v>
+      </c>
+      <c r="S119">
+        <v>0.42243822787215701</v>
+      </c>
+      <c r="T119">
+        <v>0.42221464774606599</v>
+      </c>
+      <c r="U119">
+        <v>0.42035736969492199</v>
+      </c>
+      <c r="V119">
+        <v>0.428975053407605</v>
+      </c>
+      <c r="W119">
+        <v>0.42625379396650498</v>
+      </c>
+      <c r="X119">
+        <v>0.43106947113122002</v>
+      </c>
+      <c r="Y119">
+        <v>0.42108697520713301</v>
+      </c>
+      <c r="Z119">
+        <v>0.42781016341880501</v>
+      </c>
+      <c r="AA119">
+        <v>0.428419234590944</v>
+      </c>
+      <c r="AB119">
+        <v>0.42658290085084899</v>
+      </c>
+      <c r="AC119">
+        <v>0.42422365065733197</v>
+      </c>
+      <c r="AD119">
+        <v>0.42820484715627499</v>
+      </c>
+    </row>
+    <row r="120" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>0.49667238451009199</v>
+      </c>
+      <c r="B120">
+        <v>0.490295332276594</v>
+      </c>
+      <c r="C120">
+        <v>0.48574136790969702</v>
+      </c>
+      <c r="D120">
+        <v>0.49007923327872599</v>
+      </c>
+      <c r="E120">
+        <v>0.49635746327271102</v>
+      </c>
+      <c r="F120">
+        <v>0.49180757093213201</v>
+      </c>
+      <c r="G120">
+        <v>0.49547497846109601</v>
+      </c>
+      <c r="H120">
+        <v>0.49068271430084498</v>
+      </c>
+      <c r="I120">
+        <v>0.49258718940125501</v>
+      </c>
+      <c r="J120">
+        <v>0.49384824848974501</v>
+      </c>
+      <c r="K120">
+        <v>0.49334874362134201</v>
+      </c>
+      <c r="L120">
+        <v>0.48955089783322497</v>
+      </c>
+      <c r="M120">
+        <v>0.48364511799437898</v>
+      </c>
+      <c r="N120">
+        <v>0.493134678067566</v>
+      </c>
+      <c r="O120">
+        <v>0.49521957769153901</v>
+      </c>
+      <c r="P120">
+        <v>0.49218401509896798</v>
+      </c>
+      <c r="Q120">
+        <v>0.48409167894185001</v>
+      </c>
+      <c r="R120">
+        <v>0.49618214062198202</v>
+      </c>
+      <c r="S120">
+        <v>0.49978638495426497</v>
+      </c>
+      <c r="T120">
+        <v>0.49230145700281103</v>
+      </c>
+      <c r="U120">
+        <v>0.49113450846517898</v>
+      </c>
+      <c r="V120">
+        <v>0.491874534630722</v>
+      </c>
+      <c r="W120">
+        <v>0.49423279590779301</v>
+      </c>
+      <c r="X120">
+        <v>0.49327783169276801</v>
+      </c>
+      <c r="Y120">
+        <v>0.49067939275384698</v>
+      </c>
+      <c r="Z120">
+        <v>0.492879767119979</v>
+      </c>
+      <c r="AA120">
+        <v>0.49388400455563503</v>
+      </c>
+      <c r="AB120">
+        <v>0.48844138671211601</v>
+      </c>
+      <c r="AC120">
+        <v>0.49054723860149202</v>
+      </c>
+      <c r="AD120">
+        <v>0.49580054006242302</v>
+      </c>
+    </row>
+    <row r="121" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>0.54926807572325698</v>
+      </c>
+      <c r="B121">
+        <v>0.55353301090608698</v>
+      </c>
+      <c r="C121">
+        <v>0.54675379688579395</v>
+      </c>
+      <c r="D121">
+        <v>0.54870607528327298</v>
+      </c>
+      <c r="E121">
+        <v>0.548404550484482</v>
+      </c>
+      <c r="F121">
+        <v>0.54959769191942998</v>
+      </c>
+      <c r="G121">
+        <v>0.55088856483272397</v>
+      </c>
+      <c r="H121">
+        <v>0.54945759422710905</v>
+      </c>
+      <c r="I121">
+        <v>0.55183126455332199</v>
+      </c>
+      <c r="J121">
+        <v>0.554852005889097</v>
+      </c>
+      <c r="K121">
+        <v>0.54718876090166602</v>
+      </c>
+      <c r="L121">
+        <v>0.549863765109041</v>
+      </c>
+      <c r="M121">
+        <v>0.54963923023710004</v>
+      </c>
+      <c r="N121">
+        <v>0.553382025080566</v>
+      </c>
+      <c r="O121">
+        <v>0.55166883419658697</v>
+      </c>
+      <c r="P121">
+        <v>0.54659054111183902</v>
+      </c>
+      <c r="Q121">
+        <v>0.55334959589231403</v>
+      </c>
+      <c r="R121">
+        <v>0.54857116518638105</v>
+      </c>
+      <c r="S121">
+        <v>0.55244487003368703</v>
+      </c>
+      <c r="T121">
+        <v>0.54738740770721594</v>
+      </c>
+      <c r="U121">
+        <v>0.55338908036839196</v>
+      </c>
+      <c r="V121">
+        <v>0.544462588778581</v>
+      </c>
+      <c r="W121">
+        <v>0.55175960039344896</v>
+      </c>
+      <c r="X121">
+        <v>0.55048447947845802</v>
+      </c>
+      <c r="Y121">
+        <v>0.55388361762828597</v>
+      </c>
+      <c r="Z121">
+        <v>0.55387966693471402</v>
+      </c>
+      <c r="AA121">
+        <v>0.54791540923539905</v>
+      </c>
+      <c r="AB121">
+        <v>0.54966446638877597</v>
+      </c>
+      <c r="AC121">
+        <v>0.54570482632786999</v>
+      </c>
+      <c r="AD121">
+        <v>0.547865673911062</v>
+      </c>
+    </row>
+    <row r="122" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>0.49472869136887998</v>
+      </c>
+      <c r="B122">
+        <v>0.49221466494007698</v>
+      </c>
+      <c r="C122">
+        <v>0.49847949187879098</v>
+      </c>
+      <c r="D122">
+        <v>0.50114121659489397</v>
+      </c>
+      <c r="E122">
+        <v>0.49591315926596602</v>
+      </c>
+      <c r="F122">
+        <v>0.49410955062496897</v>
+      </c>
+      <c r="G122">
+        <v>0.49394621703981301</v>
+      </c>
+      <c r="H122">
+        <v>0.496128878059094</v>
+      </c>
+      <c r="I122">
+        <v>0.49792652315975899</v>
+      </c>
+      <c r="J122">
+        <v>0.48660403503409499</v>
+      </c>
+      <c r="K122">
+        <v>0.49949426439415101</v>
+      </c>
+      <c r="L122">
+        <v>0.49223535917099998</v>
+      </c>
+      <c r="M122">
+        <v>0.49498489037284199</v>
+      </c>
+      <c r="N122">
+        <v>0.49235515091735699</v>
+      </c>
+      <c r="O122">
+        <v>0.494344268392927</v>
+      </c>
+      <c r="P122">
+        <v>0.49716794394295</v>
+      </c>
+      <c r="Q122">
+        <v>0.49806286441290798</v>
+      </c>
+      <c r="R122">
+        <v>0.49356908027569901</v>
+      </c>
+      <c r="S122">
+        <v>0.498748440958941</v>
+      </c>
+      <c r="T122">
+        <v>0.49606628666790897</v>
+      </c>
+      <c r="U122">
+        <v>0.499203126603326</v>
+      </c>
+      <c r="V122">
+        <v>0.49648525373831998</v>
+      </c>
+      <c r="W122">
+        <v>0.49352313883780502</v>
+      </c>
+      <c r="X122">
+        <v>0.49396781591580202</v>
+      </c>
+      <c r="Y122">
+        <v>0.49749177634871999</v>
+      </c>
+      <c r="Z122">
+        <v>0.49708607564658402</v>
+      </c>
+      <c r="AA122">
+        <v>0.49803722955205099</v>
+      </c>
+      <c r="AB122">
+        <v>0.49823424044023401</v>
+      </c>
+      <c r="AC122">
+        <v>0.49597107735777701</v>
+      </c>
+      <c r="AD122">
+        <v>0.49705253718548897</v>
+      </c>
+    </row>
+    <row r="123" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <f xml:space="preserve"> AVERAGE(A119:AD119)</f>
+        <v>0.42706431205967094</v>
+      </c>
+      <c r="B123">
+        <f>_xlfn.STDEV.P(A119:AD119)</f>
+        <v>3.8826723577214876E-3</v>
+      </c>
+      <c r="C123">
+        <f>_xlfn.VAR.P(A119:AD119)</f>
+        <v>1.5075144637414537E-5</v>
+      </c>
+      <c r="E123">
+        <v>1.50751446374145E-5</v>
+      </c>
+    </row>
+    <row r="124" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <f xml:space="preserve"> AVERAGE(A120:AD120)</f>
+        <v>0.49219143917209246</v>
+      </c>
+      <c r="B124">
+        <f t="shared" ref="B124:B126" si="12">_xlfn.STDEV.P(A120:AD120)</f>
+        <v>3.5394026836403003E-3</v>
+      </c>
+      <c r="C124">
+        <f t="shared" ref="C124:E126" si="13">_xlfn.VAR.P(A120:AD120)</f>
+        <v>1.2527371356960161E-5</v>
+      </c>
+      <c r="E124">
+        <v>1.2527371356960199E-5</v>
+      </c>
+    </row>
+    <row r="125" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <f xml:space="preserve"> AVERAGE(A121:AD121)</f>
+        <v>0.55007960785353205</v>
+      </c>
+      <c r="B125">
+        <f t="shared" si="12"/>
+        <v>2.7004076060301307E-3</v>
+      </c>
+      <c r="C125">
+        <f>_xlfn.VAR.P(A121:AD121)</f>
+        <v>7.2922012387053826E-6</v>
+      </c>
+      <c r="E125">
+        <v>7.2922012387053826E-6</v>
+      </c>
+    </row>
+    <row r="126" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <f xml:space="preserve"> AVERAGE(A122:AD122)</f>
+        <v>0.49584244163663771</v>
+      </c>
+      <c r="B126">
+        <f t="shared" si="12"/>
+        <v>2.8550198207913349E-3</v>
+      </c>
+      <c r="C126">
+        <f t="shared" si="13"/>
+        <v>8.151138177111387E-6</v>
+      </c>
+      <c r="E126">
+        <v>8.151138177111387E-6</v>
+      </c>
+    </row>
+    <row r="130" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="131" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>0.82719550919826501</v>
+      </c>
+      <c r="B131">
+        <v>0.81455904402948198</v>
+      </c>
+      <c r="C131">
+        <v>0.81676833887370104</v>
+      </c>
+      <c r="D131">
+        <v>0.80765860522831601</v>
+      </c>
+      <c r="E131">
+        <v>0.82042598065571304</v>
+      </c>
+      <c r="F131">
+        <v>0.80232221980894702</v>
+      </c>
+      <c r="G131">
+        <v>0.81299575839722005</v>
+      </c>
+      <c r="H131">
+        <v>0.81089010669797101</v>
+      </c>
+      <c r="I131">
+        <v>0.81377524610896901</v>
+      </c>
+      <c r="J131">
+        <v>0.81538164877367403</v>
+      </c>
+      <c r="K131">
+        <v>0.81087225960541598</v>
+      </c>
+      <c r="L131">
+        <v>0.81484264582928601</v>
+      </c>
+      <c r="M131">
+        <v>0.81690547626376098</v>
+      </c>
+      <c r="N131">
+        <v>0.795749041389337</v>
+      </c>
+      <c r="O131">
+        <v>0.81785558899932598</v>
+      </c>
+      <c r="P131">
+        <v>0.81327391589632303</v>
+      </c>
+      <c r="Q131">
+        <v>0.81898386073382301</v>
+      </c>
+      <c r="R131">
+        <v>0.81620457307321903</v>
+      </c>
+      <c r="S131">
+        <v>0.79554691184126303</v>
+      </c>
+      <c r="T131">
+        <v>0.82564034356434701</v>
+      </c>
+    </row>
+    <row r="132" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>0.85839042222845596</v>
+      </c>
+      <c r="B132">
+        <v>0.85093657137031398</v>
+      </c>
+      <c r="C132">
+        <v>0.84001113301708696</v>
+      </c>
+      <c r="D132">
+        <v>0.85795485515056202</v>
+      </c>
+      <c r="E132">
+        <v>0.85560017956678802</v>
+      </c>
+      <c r="F132">
+        <v>0.83168809402236898</v>
+      </c>
+      <c r="G132">
+        <v>0.82280205075595703</v>
+      </c>
+      <c r="H132">
+        <v>0.84595379779950197</v>
+      </c>
+      <c r="I132">
+        <v>0.85858744204688298</v>
+      </c>
+      <c r="J132">
+        <v>0.86066160537095704</v>
+      </c>
+      <c r="K132">
+        <v>0.84244611599981001</v>
+      </c>
+      <c r="L132">
+        <v>0.84975689394735499</v>
+      </c>
+      <c r="M132">
+        <v>0.84140365872119405</v>
+      </c>
+      <c r="N132">
+        <v>0.85896297316744896</v>
+      </c>
+      <c r="O132">
+        <v>0.82918199013328597</v>
+      </c>
+      <c r="P132">
+        <v>0.85483284769553602</v>
+      </c>
+      <c r="Q132">
+        <v>0.85775193183085496</v>
+      </c>
+      <c r="R132">
+        <v>0.85499671870181104</v>
+      </c>
+      <c r="S132">
+        <v>0.86306995524011998</v>
+      </c>
+      <c r="T132">
+        <v>0.84680583002103804</v>
+      </c>
+    </row>
+    <row r="133" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>0.83233469355448197</v>
+      </c>
+      <c r="B133">
+        <v>0.83337555772634797</v>
+      </c>
+      <c r="C133">
+        <v>0.83876185687097504</v>
+      </c>
+      <c r="D133">
+        <v>0.82851444594857704</v>
+      </c>
+      <c r="E133">
+        <v>0.82371451585431199</v>
+      </c>
+      <c r="F133">
+        <v>0.83535051284397699</v>
+      </c>
+      <c r="G133">
+        <v>0.82674539620524201</v>
+      </c>
+      <c r="H133">
+        <v>0.82969843554902301</v>
+      </c>
+      <c r="I133">
+        <v>0.82270602072080401</v>
+      </c>
+      <c r="J133">
+        <v>0.81774818844881103</v>
+      </c>
+      <c r="K133">
+        <v>0.84048024615768302</v>
+      </c>
+      <c r="L133">
+        <v>0.84129057539062502</v>
+      </c>
+      <c r="M133">
+        <v>0.82551482032822598</v>
+      </c>
+      <c r="N133">
+        <v>0.84395161359924697</v>
+      </c>
+      <c r="O133">
+        <v>0.83021557674603796</v>
+      </c>
+      <c r="P133">
+        <v>0.83611502752893796</v>
+      </c>
+      <c r="Q133">
+        <v>0.85641487291414597</v>
+      </c>
+      <c r="R133">
+        <v>0.83480960741168997</v>
+      </c>
+      <c r="S133">
+        <v>0.83627609243671797</v>
+      </c>
+      <c r="T133">
+        <v>0.83340158681969401</v>
+      </c>
+    </row>
+    <row r="134" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>0.64975059876906704</v>
+      </c>
+      <c r="B134">
+        <v>0.654902817930333</v>
+      </c>
+      <c r="C134">
+        <v>0.68569621567588901</v>
+      </c>
+      <c r="D134">
+        <v>0.64653724156110504</v>
+      </c>
+      <c r="E134">
+        <v>0.65380802575172103</v>
+      </c>
+      <c r="F134">
+        <v>0.62663355997078696</v>
+      </c>
+      <c r="G134">
+        <v>0.67163007867837499</v>
+      </c>
+      <c r="H134">
+        <v>0.66843926492346595</v>
+      </c>
+      <c r="I134">
+        <v>0.671717018545125</v>
+      </c>
+      <c r="J134">
+        <v>0.65242727668977496</v>
+      </c>
+      <c r="K134">
+        <v>0.64372543006015304</v>
+      </c>
+      <c r="L134">
+        <v>0.64650186796068998</v>
+      </c>
+      <c r="M134">
+        <v>0.695289094064378</v>
+      </c>
+      <c r="N134">
+        <v>0.64711653470724795</v>
+      </c>
+      <c r="O134">
+        <v>0.63831420193673905</v>
+      </c>
+      <c r="P134">
+        <v>0.69299552654864804</v>
+      </c>
+      <c r="Q134">
+        <v>0.66057521529893004</v>
+      </c>
+      <c r="R134">
+        <v>0.65958070294730697</v>
+      </c>
+      <c r="S134">
+        <v>0.65506116806639603</v>
+      </c>
+      <c r="T134">
+        <v>0.66441284564107805</v>
+      </c>
+    </row>
+    <row r="135" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <f>AVERAGE(A131:T131)</f>
+        <v>0.81339235374841812</v>
+      </c>
+      <c r="B135">
+        <f>_xlfn.STDEV.P(A131:T131)</f>
+        <v>7.9948965431740106E-3</v>
+      </c>
+      <c r="C135">
+        <f>_xlfn.VAR.P(A131:T131)</f>
+        <v>6.3918370736055753E-5</v>
+      </c>
+    </row>
+    <row r="136" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <f>AVERAGE(A132:T132)</f>
+        <v>0.8490897533393662</v>
+      </c>
+      <c r="B136">
+        <f t="shared" ref="B136:B138" si="14">_xlfn.STDEV.P(A132:T132)</f>
+        <v>1.1095379525631948E-2</v>
+      </c>
+      <c r="C136">
+        <f>_xlfn.VAR.P(A132:T132)</f>
+        <v>1.2310744681781263E-4</v>
+      </c>
+    </row>
+    <row r="137" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <f>AVERAGE(A133:T133)</f>
+        <v>0.83337098215277783</v>
+      </c>
+      <c r="B137">
+        <f t="shared" si="14"/>
+        <v>8.4024832411584705E-3</v>
+      </c>
+      <c r="C137">
+        <f>_xlfn.VAR.P(A133:T133)</f>
+        <v>7.0601724617948961E-5</v>
+      </c>
+    </row>
+    <row r="138" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <f t="shared" ref="A136:A138" si="15">AVERAGE(A134:T134)</f>
+        <v>0.65925573428636042</v>
+      </c>
+      <c r="B138">
+        <f t="shared" si="14"/>
+        <v>1.7285809598253658E-2</v>
+      </c>
+      <c r="C138">
+        <f t="shared" ref="C136:C138" si="16">_xlfn.VAR.P(A134:T134)</f>
+        <v>2.9879921346707831E-4</v>
+      </c>
+    </row>
+    <row r="141" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="142" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>0.80662396907912703</v>
+      </c>
+      <c r="B142">
+        <v>0.77746135144601303</v>
+      </c>
+      <c r="C142">
+        <v>0.79688032241131701</v>
+      </c>
+      <c r="D142">
+        <v>0.79146630720798605</v>
+      </c>
+      <c r="E142">
+        <v>0.79899952599386403</v>
+      </c>
+      <c r="F142">
+        <v>0.79684431862054805</v>
+      </c>
+      <c r="G142">
+        <v>0.80126044284651898</v>
+      </c>
+      <c r="H142">
+        <v>0.78127536380112295</v>
+      </c>
+      <c r="I142">
+        <v>0.78986539876386197</v>
+      </c>
+      <c r="J142">
+        <v>0.79323177086265095</v>
+      </c>
+      <c r="K142">
+        <v>0.78951058973294097</v>
+      </c>
+      <c r="L142">
+        <v>0.79622684711918101</v>
+      </c>
+      <c r="M142">
+        <v>0.76283251635481097</v>
+      </c>
+      <c r="N142">
+        <v>0.80041342691661099</v>
+      </c>
+      <c r="O142">
+        <v>0.79912604528661502</v>
+      </c>
+      <c r="P142">
+        <v>0.76470626720424995</v>
+      </c>
+      <c r="Q142">
+        <v>0.77774057486352</v>
+      </c>
+      <c r="R142">
+        <v>0.77177380734779399</v>
+      </c>
+      <c r="S142">
+        <v>0.79202366251484801</v>
+      </c>
+      <c r="T142">
+        <v>0.78571110630539698</v>
+      </c>
+    </row>
+    <row r="143" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>0.863955568975185</v>
+      </c>
+      <c r="B143">
+        <v>0.85501256731571895</v>
+      </c>
+      <c r="C143">
+        <v>0.86195686719333897</v>
+      </c>
+      <c r="D143">
+        <v>0.84559265270237305</v>
+      </c>
+      <c r="E143">
+        <v>0.867117487606337</v>
+      </c>
+      <c r="F143">
+        <v>0.84835988413721897</v>
+      </c>
+      <c r="G143">
+        <v>0.85675022492283104</v>
+      </c>
+      <c r="H143">
+        <v>0.858620663702651</v>
+      </c>
+      <c r="I143">
+        <v>0.86243301428977603</v>
+      </c>
+      <c r="J143">
+        <v>0.85952925230709198</v>
+      </c>
+      <c r="K143">
+        <v>0.86298509191498696</v>
+      </c>
+      <c r="L143">
+        <v>0.85891974030473095</v>
+      </c>
+      <c r="M143">
+        <v>0.85805837842802701</v>
+      </c>
+      <c r="N143">
+        <v>0.87712987195260905</v>
+      </c>
+      <c r="O143">
+        <v>0.859829837965432</v>
+      </c>
+      <c r="P143">
+        <v>0.86541272418078996</v>
+      </c>
+      <c r="Q143">
+        <v>0.87068775518689701</v>
+      </c>
+      <c r="R143">
+        <v>0.86018736459579304</v>
+      </c>
+      <c r="S143">
+        <v>0.858408475396927</v>
+      </c>
+      <c r="T143">
+        <v>0.84089820305918495</v>
+      </c>
+    </row>
+    <row r="144" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>0.88078732217393996</v>
+      </c>
+      <c r="B144">
+        <v>0.87463561837109205</v>
+      </c>
+      <c r="C144">
+        <v>0.88303015979035304</v>
+      </c>
+      <c r="D144">
+        <v>0.87151410445114097</v>
+      </c>
+      <c r="E144">
+        <v>0.88151779824237797</v>
+      </c>
+      <c r="F144">
+        <v>0.88655743195376702</v>
+      </c>
+      <c r="G144">
+        <v>0.87728888605907795</v>
+      </c>
+      <c r="H144">
+        <v>0.88552632754796101</v>
+      </c>
+      <c r="I144">
+        <v>0.88204468295024496</v>
+      </c>
+      <c r="J144">
+        <v>0.88097603050460005</v>
+      </c>
+      <c r="K144">
+        <v>0.88127606592766805</v>
+      </c>
+      <c r="L144">
+        <v>0.87179789936377805</v>
+      </c>
+      <c r="M144">
+        <v>0.86741830160470601</v>
+      </c>
+      <c r="N144">
+        <v>0.89646253540842202</v>
+      </c>
+      <c r="O144">
+        <v>0.88838629032606198</v>
+      </c>
+      <c r="P144">
+        <v>0.87536020489056299</v>
+      </c>
+      <c r="Q144">
+        <v>0.87381827732891304</v>
+      </c>
+      <c r="R144">
+        <v>0.89358699550930998</v>
+      </c>
+      <c r="S144">
+        <v>0.89329609062215298</v>
+      </c>
+      <c r="T144">
+        <v>0.86240199468911705</v>
+      </c>
+    </row>
+    <row r="145" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>0.84794837983256999</v>
+      </c>
+      <c r="B145">
+        <v>0.83233809080802101</v>
+      </c>
+      <c r="C145">
+        <v>0.831766991640566</v>
+      </c>
+      <c r="D145">
+        <v>0.84179859300382898</v>
+      </c>
+      <c r="E145">
+        <v>0.84052936013409796</v>
+      </c>
+      <c r="F145">
+        <v>0.84744214999561296</v>
+      </c>
+      <c r="G145">
+        <v>0.84014084724389904</v>
+      </c>
+      <c r="H145">
+        <v>0.84235694665817695</v>
+      </c>
+      <c r="I145">
+        <v>0.84018742913944899</v>
+      </c>
+      <c r="J145">
+        <v>0.85949461063552202</v>
+      </c>
+      <c r="K145">
+        <v>0.85651354154555104</v>
+      </c>
+      <c r="L145">
+        <v>0.83809983617016504</v>
+      </c>
+      <c r="M145">
+        <v>0.852182071113184</v>
+      </c>
+      <c r="N145">
+        <v>0.83011706676653696</v>
+      </c>
+      <c r="O145">
+        <v>0.82993468596961495</v>
+      </c>
+      <c r="P145">
+        <v>0.838343164018446</v>
+      </c>
+      <c r="Q145">
+        <v>0.82259637516200701</v>
+      </c>
+      <c r="R145">
+        <v>0.835289621249662</v>
+      </c>
+      <c r="S145">
+        <v>0.84541179583423398</v>
+      </c>
+      <c r="T145">
+        <v>0.84137485986494898</v>
+      </c>
+    </row>
+    <row r="146" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <f>AVERAGE(A142:T142)</f>
+        <v>0.78869868073394889</v>
+      </c>
+      <c r="B146">
+        <f>_xlfn.STDEV.P(A142:T142)</f>
+        <v>1.2049833208120081E-2</v>
+      </c>
+      <c r="C146">
+        <f>_xlfn.VAR.P(A142:T142)</f>
+        <v>1.4519848034351347E-4</v>
+      </c>
+    </row>
+    <row r="147" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <f>AVERAGE(A143:T143)</f>
+        <v>0.85959228130689502</v>
+      </c>
+      <c r="B147">
+        <f>_xlfn.STDEV.P(A143:T143)</f>
+        <v>7.9738149428544725E-3</v>
+      </c>
+      <c r="C147">
+        <f t="shared" ref="C147:C149" si="17">_xlfn.VAR.P(A143:T143)</f>
+        <v>6.3581724742889278E-5</v>
+      </c>
+    </row>
+    <row r="148" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <f t="shared" ref="A147:A149" si="18">AVERAGE(A144:T144)</f>
+        <v>0.88038415088576227</v>
+      </c>
+      <c r="B148">
+        <f t="shared" ref="B147:B149" si="19">_xlfn.STDEV.P(A144:T144)</f>
+        <v>8.646777645226698E-3</v>
+      </c>
+      <c r="C148">
+        <f t="shared" si="17"/>
+        <v>7.4766763645992153E-5</v>
+      </c>
+    </row>
+    <row r="149" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <f t="shared" si="18"/>
+        <v>0.8406933208393047</v>
+      </c>
+      <c r="B149">
+        <f>_xlfn.STDEV.P(A145:T145)</f>
+        <v>8.9646278896434485E-3</v>
+      </c>
+      <c r="C149">
+        <f t="shared" si="17"/>
+        <v>8.0364553199773145E-5</v>
+      </c>
+    </row>
+    <row r="152" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="153" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>0.57006648854560804</v>
+      </c>
+      <c r="B153">
+        <v>0.57129764274706496</v>
+      </c>
+      <c r="C153">
+        <v>0.57527652955730801</v>
+      </c>
+      <c r="D153">
+        <v>0.573145193385313</v>
+      </c>
+      <c r="E153">
+        <v>0.56583520472438598</v>
+      </c>
+      <c r="F153">
+        <v>0.57423042741386299</v>
+      </c>
+      <c r="G153">
+        <v>0.57683548960919895</v>
+      </c>
+      <c r="H153">
+        <v>0.57914193763739596</v>
+      </c>
+      <c r="I153">
+        <v>0.57292187308307396</v>
+      </c>
+      <c r="J153">
+        <v>0.57779449514831105</v>
+      </c>
+      <c r="K153">
+        <v>0.56879002439137205</v>
+      </c>
+      <c r="L153">
+        <v>0.56686715897186801</v>
+      </c>
+      <c r="M153">
+        <v>0.57182456757248201</v>
+      </c>
+      <c r="N153">
+        <v>0.56834415325355103</v>
+      </c>
+      <c r="O153">
+        <v>0.57874671678325096</v>
+      </c>
+      <c r="P153">
+        <v>0.57356726861351803</v>
+      </c>
+      <c r="Q153">
+        <v>0.57747894026219104</v>
+      </c>
+      <c r="R153">
+        <v>0.57098112190046402</v>
+      </c>
+      <c r="S153">
+        <v>0.56762468365593799</v>
+      </c>
+      <c r="T153">
+        <v>0.56861028851231499</v>
+      </c>
+    </row>
+    <row r="154" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>0.63403122003110202</v>
+      </c>
+      <c r="B154">
+        <v>0.62745966281895305</v>
+      </c>
+      <c r="C154">
+        <v>0.64221904933935803</v>
+      </c>
+      <c r="D154">
+        <v>0.64066580703221898</v>
+      </c>
+      <c r="E154">
+        <v>0.64200276718818805</v>
+      </c>
+      <c r="F154">
+        <v>0.63184722815276995</v>
+      </c>
+      <c r="G154">
+        <v>0.63018809231776196</v>
+      </c>
+      <c r="H154">
+        <v>0.63347866171911504</v>
+      </c>
+      <c r="I154">
+        <v>0.63569667864017398</v>
+      </c>
+      <c r="J154">
+        <v>0.63005784538165499</v>
+      </c>
+      <c r="K154">
+        <v>0.64197063901387397</v>
+      </c>
+      <c r="L154">
+        <v>0.63258715735662396</v>
+      </c>
+      <c r="M154">
+        <v>0.62714893339668498</v>
+      </c>
+      <c r="N154">
+        <v>0.63393263184447501</v>
+      </c>
+      <c r="O154">
+        <v>0.63591411508061602</v>
+      </c>
+      <c r="P154">
+        <v>0.632027062688025</v>
+      </c>
+      <c r="Q154">
+        <v>0.63367347964454401</v>
+      </c>
+      <c r="R154">
+        <v>0.63601295509034905</v>
+      </c>
+      <c r="S154">
+        <v>0.62743060958609798</v>
+      </c>
+      <c r="T154">
+        <v>0.632826536555119</v>
+      </c>
+    </row>
+    <row r="155" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>0.69399128819074396</v>
+      </c>
+      <c r="B155">
+        <v>0.68636387412405597</v>
+      </c>
+      <c r="C155">
+        <v>0.68819317659494295</v>
+      </c>
+      <c r="D155">
+        <v>0.69431145556949603</v>
+      </c>
+      <c r="E155">
+        <v>0.69486106659142099</v>
+      </c>
+      <c r="F155">
+        <v>0.69312663078158099</v>
+      </c>
+      <c r="G155">
+        <v>0.69286619051130405</v>
+      </c>
+      <c r="H155">
+        <v>0.69024957339003601</v>
+      </c>
+      <c r="I155">
+        <v>0.69565277413543403</v>
+      </c>
+      <c r="J155">
+        <v>0.69410039916452704</v>
+      </c>
+      <c r="K155">
+        <v>0.69124226622155405</v>
+      </c>
+      <c r="L155">
+        <v>0.69347239798101001</v>
+      </c>
+      <c r="M155">
+        <v>0.69281860441709897</v>
+      </c>
+      <c r="N155">
+        <v>0.69354590351782397</v>
+      </c>
+      <c r="O155">
+        <v>0.697255129908113</v>
+      </c>
+      <c r="P155">
+        <v>0.694365215535512</v>
+      </c>
+      <c r="Q155">
+        <v>0.69477100862148</v>
+      </c>
+      <c r="R155">
+        <v>0.69446509191442196</v>
+      </c>
+      <c r="S155">
+        <v>0.69468826325993804</v>
+      </c>
+      <c r="T155">
+        <v>0.68928808936694397</v>
+      </c>
+    </row>
+    <row r="156" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>0.63768674672720604</v>
+      </c>
+      <c r="B156">
+        <v>0.63702630261233895</v>
+      </c>
+      <c r="C156">
+        <v>0.63132709311881197</v>
+      </c>
+      <c r="D156">
+        <v>0.63405630095919097</v>
+      </c>
+      <c r="E156">
+        <v>0.63571610363408904</v>
+      </c>
+      <c r="F156">
+        <v>0.63312935644342405</v>
+      </c>
+      <c r="G156">
+        <v>0.63614412579104695</v>
+      </c>
+      <c r="H156">
+        <v>0.63942295498138202</v>
+      </c>
+      <c r="I156">
+        <v>0.63837480178539097</v>
+      </c>
+      <c r="J156">
+        <v>0.63602086704781902</v>
+      </c>
+      <c r="K156">
+        <v>0.64210145875664304</v>
+      </c>
+      <c r="L156">
+        <v>0.63519563660960598</v>
+      </c>
+      <c r="M156">
+        <v>0.64405533139504201</v>
+      </c>
+      <c r="N156">
+        <v>0.63408149099801703</v>
+      </c>
+      <c r="O156">
+        <v>0.63369751421949505</v>
+      </c>
+      <c r="P156">
+        <v>0.636116338922744</v>
+      </c>
+      <c r="Q156">
+        <v>0.63644921620776995</v>
+      </c>
+      <c r="R156">
+        <v>0.64149986286404803</v>
+      </c>
+      <c r="S156">
+        <v>0.64026580831402202</v>
+      </c>
+      <c r="T156">
+        <v>0.64105184420624295</v>
+      </c>
+    </row>
+    <row r="157" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <f>AVERAGE(A153:T153)</f>
+        <v>0.57246901028842367</v>
+      </c>
+      <c r="B157">
+        <f>_xlfn.STDEV.P(A153:T153)</f>
+        <v>4.0211017396353712E-3</v>
+      </c>
+      <c r="C157">
+        <f>_xlfn.VAR.P(A153:T153)</f>
+        <v>1.616925920049861E-5</v>
+      </c>
+      <c r="E157">
+        <v>1.61692592004986E-5</v>
+      </c>
+    </row>
+    <row r="158" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <f t="shared" ref="A158:A160" si="20">AVERAGE(A154:T154)</f>
+        <v>0.63405855664388522</v>
+      </c>
+      <c r="B158">
+        <f t="shared" ref="B158:B160" si="21">_xlfn.STDEV.P(A154:T154)</f>
+        <v>4.6114655964948816E-3</v>
+      </c>
+      <c r="C158">
+        <f t="shared" ref="C158:C160" si="22">_xlfn.VAR.P(A154:T154)</f>
+        <v>2.1265614947655898E-5</v>
+      </c>
+      <c r="E158">
+        <v>2.1265614947655901E-5</v>
+      </c>
+    </row>
+    <row r="159" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <f t="shared" si="20"/>
+        <v>0.69298141998987184</v>
+      </c>
+      <c r="B159">
+        <f t="shared" si="21"/>
+        <v>2.5949465537107447E-3</v>
+      </c>
+      <c r="C159">
+        <f t="shared" si="22"/>
+        <v>6.7337476166152715E-6</v>
+      </c>
+      <c r="E159" s="1">
+        <v>6.7337476166152698E-6</v>
+      </c>
+    </row>
+    <row r="160" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <f t="shared" si="20"/>
+        <v>0.63717095777971655</v>
+      </c>
+      <c r="B160">
+        <f t="shared" si="21"/>
+        <v>3.2689115175212561E-3</v>
+      </c>
+      <c r="C160">
+        <f t="shared" si="22"/>
+        <v>1.068578250938312E-5</v>
+      </c>
+      <c r="E160">
+        <v>1.06857825093831E-5</v>
+      </c>
+    </row>
+    <row r="165" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="166" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A166">
+        <v>0.78197241613214596</v>
+      </c>
+      <c r="B166">
+        <v>0.78654816980476205</v>
+      </c>
+      <c r="C166">
+        <v>0.78228522432061698</v>
+      </c>
+      <c r="D166">
+        <v>0.77308099295504895</v>
+      </c>
+      <c r="E166">
+        <v>0.76307427925092197</v>
+      </c>
+      <c r="F166">
+        <v>0.78040379574015195</v>
+      </c>
+      <c r="G166">
+        <v>0.78909098450339099</v>
+      </c>
+      <c r="H166">
+        <v>0.80175559113833605</v>
+      </c>
+      <c r="I166">
+        <v>0.77339175356202905</v>
+      </c>
+      <c r="J166">
+        <v>0.78430015650283802</v>
+      </c>
+      <c r="K166">
+        <v>0.77158816904733696</v>
+      </c>
+      <c r="L166">
+        <v>0.79257547402100503</v>
+      </c>
+      <c r="M166">
+        <v>0.79722922717843203</v>
+      </c>
+      <c r="N166">
+        <v>0.76116294254622696</v>
+      </c>
+      <c r="O166">
+        <v>0.78226247059026099</v>
+      </c>
+      <c r="P166">
+        <v>0.80347509407572104</v>
+      </c>
+      <c r="Q166">
+        <v>0.784406830523799</v>
+      </c>
+      <c r="R166">
+        <v>0.79308587669060704</v>
+      </c>
+      <c r="S166">
+        <v>0.77522899713310001</v>
+      </c>
+      <c r="T166">
+        <v>0.773745908510311</v>
+      </c>
+    </row>
+    <row r="167" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A167">
+        <v>0.86087124274437599</v>
+      </c>
+      <c r="B167">
+        <v>0.84944640037521302</v>
+      </c>
+      <c r="C167">
+        <v>0.85222705795388798</v>
+      </c>
+      <c r="D167">
+        <v>0.86863531943277905</v>
+      </c>
+      <c r="E167">
+        <v>0.86433935659485495</v>
+      </c>
+      <c r="F167">
+        <v>0.86185219315204198</v>
+      </c>
+      <c r="G167">
+        <v>0.85743203183051997</v>
+      </c>
+      <c r="H167">
+        <v>0.85580252064365703</v>
+      </c>
+      <c r="I167">
+        <v>0.87553357647954699</v>
+      </c>
+      <c r="J167">
+        <v>0.85268628983331896</v>
+      </c>
+      <c r="K167">
+        <v>0.85631512992441206</v>
+      </c>
+      <c r="L167">
+        <v>0.87916889545472499</v>
+      </c>
+      <c r="M167">
+        <v>0.86337001669953894</v>
+      </c>
+      <c r="N167">
+        <v>0.85961712809118096</v>
+      </c>
+      <c r="O167">
+        <v>0.85887470414739597</v>
+      </c>
+      <c r="P167">
+        <v>0.86820175265645905</v>
+      </c>
+      <c r="Q167">
+        <v>0.86388696935839804</v>
+      </c>
+      <c r="R167">
+        <v>0.85826340951110502</v>
+      </c>
+      <c r="S167">
+        <v>0.86383595311926298</v>
+      </c>
+      <c r="T167">
+        <v>0.86080937146763703</v>
+      </c>
+    </row>
+    <row r="168" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A168">
+        <v>0.88820131128640301</v>
+      </c>
+      <c r="B168">
+        <v>0.89290643100886002</v>
+      </c>
+      <c r="C168">
+        <v>0.88395172337464401</v>
+      </c>
+      <c r="D168">
+        <v>0.88966122985983398</v>
+      </c>
+      <c r="E168">
+        <v>0.89390910287106595</v>
+      </c>
+      <c r="F168">
+        <v>0.88768811041474605</v>
+      </c>
+      <c r="G168">
+        <v>0.88507693407918597</v>
+      </c>
+      <c r="H168">
+        <v>0.89591297076432796</v>
+      </c>
+      <c r="I168">
+        <v>0.89694579177088496</v>
+      </c>
+      <c r="J168">
+        <v>0.88111896025172698</v>
+      </c>
+      <c r="K168">
+        <v>0.884720154490379</v>
+      </c>
+      <c r="L168">
+        <v>0.90727508678852498</v>
+      </c>
+      <c r="M168">
+        <v>0.87587830327094396</v>
+      </c>
+      <c r="N168">
+        <v>0.88771658900123696</v>
+      </c>
+      <c r="O168">
+        <v>0.87922260530731</v>
+      </c>
+      <c r="P168">
+        <v>0.88044507358857804</v>
+      </c>
+      <c r="Q168">
+        <v>0.89402317791622599</v>
+      </c>
+      <c r="R168">
+        <v>0.89204104490237102</v>
+      </c>
+      <c r="S168">
+        <v>0.88994931518193199</v>
+      </c>
+      <c r="T168">
+        <v>0.89518208695314605</v>
+      </c>
+    </row>
+    <row r="169" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A169">
+        <v>0.86824791745259</v>
+      </c>
+      <c r="B169">
+        <v>0.88046611306451605</v>
+      </c>
+      <c r="C169">
+        <v>0.88354003281313098</v>
+      </c>
+      <c r="D169">
+        <v>0.87616512637724597</v>
+      </c>
+      <c r="E169">
+        <v>0.86870443967575595</v>
+      </c>
+      <c r="F169">
+        <v>0.88361642397981699</v>
+      </c>
+      <c r="G169">
+        <v>0.866328855653138</v>
+      </c>
+      <c r="H169">
+        <v>0.882142605642944</v>
+      </c>
+      <c r="I169">
+        <v>0.87335680308378905</v>
+      </c>
+      <c r="J169">
+        <v>0.87799439389560696</v>
+      </c>
+      <c r="K169">
+        <v>0.86332677369405098</v>
+      </c>
+      <c r="L169">
+        <v>0.87578068964870903</v>
+      </c>
+      <c r="M169">
+        <v>0.88072007898240801</v>
+      </c>
+      <c r="N169">
+        <v>0.87209325528780901</v>
+      </c>
+      <c r="O169">
+        <v>0.87203869145203095</v>
+      </c>
+      <c r="P169">
+        <v>0.87999500039870204</v>
+      </c>
+      <c r="Q169">
+        <v>0.87768482000228598</v>
+      </c>
+      <c r="R169">
+        <v>0.88538718131574901</v>
+      </c>
+      <c r="S169">
+        <v>0.87621123613028495</v>
+      </c>
+      <c r="T169">
+        <v>0.87924729488759601</v>
+      </c>
+    </row>
+    <row r="170" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A170">
+        <f>AVERAGE(A166:T166)</f>
+        <v>0.78253321771135209</v>
+      </c>
+      <c r="B170">
+        <f>_xlfn.STDEV.P(A166:T166)</f>
+        <v>1.1326060271632051E-2</v>
+      </c>
+      <c r="C170">
+        <f>_xlfn.VAR.P(A166:T166)</f>
+        <v>1.2827964127664189E-4</v>
+      </c>
+      <c r="E170">
+        <v>1.2827964127664189E-4</v>
+      </c>
+    </row>
+    <row r="171" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A171">
+        <f>AVERAGE(A167:T167)</f>
+        <v>0.86155846597351571</v>
+      </c>
+      <c r="B171">
+        <f t="shared" ref="B171:B173" si="23">_xlfn.STDEV.P(A167:T167)</f>
+        <v>7.1915304881889795E-3</v>
+      </c>
+      <c r="C171">
+        <f t="shared" ref="C171:C173" si="24">_xlfn.VAR.P(A167:T167)</f>
+        <v>5.1718110762551625E-5</v>
+      </c>
+      <c r="E171">
+        <v>5.1718110762551598E-5</v>
+      </c>
+    </row>
+    <row r="172" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <f>AVERAGE(A168:T168)</f>
+        <v>0.88909130015411653</v>
+      </c>
+      <c r="B172">
+        <f t="shared" si="23"/>
+        <v>7.1568355099630512E-3</v>
+      </c>
+      <c r="C172">
+        <f t="shared" si="24"/>
+        <v>5.1220294516668094E-5</v>
+      </c>
+      <c r="E172">
+        <v>5.12202945166681E-5</v>
+      </c>
+    </row>
+    <row r="173" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A173">
+        <f t="shared" ref="A171:A173" si="25">AVERAGE(A169:T169)</f>
+        <v>0.87615238667190809</v>
+      </c>
+      <c r="B173">
+        <f t="shared" si="23"/>
+        <v>6.0054875646031285E-3</v>
+      </c>
+      <c r="C173">
+        <f t="shared" si="24"/>
+        <v>3.6065880888602819E-5</v>
+      </c>
+      <c r="E173">
+        <v>3.6065880888602798E-5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>